<commit_message>
avance hasta el cuadro de la regresion hecha
</commit_message>
<xml_diff>
--- a/base_datos/PBIMINERO.xlsx
+++ b/base_datos/PBIMINERO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\finalKoyck\base_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6357B633-4267-4396-A342-73DD766AC572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD15EE33-872E-4A9B-9930-4B6AAC4760C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{E9A4BC18-0E6E-4B76-8B5A-933A70F10F7C}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="10110" windowHeight="9270" xr2:uid="{E9A4BC18-0E6E-4B76-8B5A-933A70F10F7C}"/>
   </bookViews>
   <sheets>
     <sheet name="pbisectorminero" sheetId="11" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B1" sqref="B1:C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finalizando el trabajo final de Koyck, solo falta revisión final
</commit_message>
<xml_diff>
--- a/base_datos/PBIMINERO.xlsx
+++ b/base_datos/PBIMINERO.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\finalKoyck\base_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD15EE33-872E-4A9B-9930-4B6AAC4760C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967A2F64-F8E4-43E9-9DD1-2E2F444D737E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="10110" windowHeight="9270" xr2:uid="{E9A4BC18-0E6E-4B76-8B5A-933A70F10F7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{E9A4BC18-0E6E-4B76-8B5A-933A70F10F7C}"/>
   </bookViews>
   <sheets>
-    <sheet name="pbisectorminero" sheetId="11" r:id="rId1"/>
+    <sheet name="pbisectorminero" sheetId="12" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>mes</t>
   </si>
@@ -59,6 +59,297 @@
   </si>
   <si>
     <t>pbiminero</t>
+  </si>
+  <si>
+    <t>2002M01</t>
+  </si>
+  <si>
+    <t>2002M02</t>
+  </si>
+  <si>
+    <t>2002M03</t>
+  </si>
+  <si>
+    <t>2002M04</t>
+  </si>
+  <si>
+    <t>2002M05</t>
+  </si>
+  <si>
+    <t>2002M06</t>
+  </si>
+  <si>
+    <t>2002M07</t>
+  </si>
+  <si>
+    <t>2002M08</t>
+  </si>
+  <si>
+    <t>2002M09</t>
+  </si>
+  <si>
+    <t>2002M10</t>
+  </si>
+  <si>
+    <t>2002M11</t>
+  </si>
+  <si>
+    <t>2002M12</t>
+  </si>
+  <si>
+    <t>2003M01</t>
+  </si>
+  <si>
+    <t>2003M02</t>
+  </si>
+  <si>
+    <t>2003M03</t>
+  </si>
+  <si>
+    <t>2003M04</t>
+  </si>
+  <si>
+    <t>2003M05</t>
+  </si>
+  <si>
+    <t>2003M06</t>
+  </si>
+  <si>
+    <t>2003M07</t>
+  </si>
+  <si>
+    <t>2003M08</t>
+  </si>
+  <si>
+    <t>2003M09</t>
+  </si>
+  <si>
+    <t>2003M10</t>
+  </si>
+  <si>
+    <t>2003M11</t>
+  </si>
+  <si>
+    <t>2003M12</t>
+  </si>
+  <si>
+    <t>2004M01</t>
+  </si>
+  <si>
+    <t>2004M02</t>
+  </si>
+  <si>
+    <t>2004M03</t>
+  </si>
+  <si>
+    <t>2004M04</t>
+  </si>
+  <si>
+    <t>2004M05</t>
+  </si>
+  <si>
+    <t>2004M06</t>
+  </si>
+  <si>
+    <t>2004M07</t>
+  </si>
+  <si>
+    <t>2004M08</t>
+  </si>
+  <si>
+    <t>2004M09</t>
+  </si>
+  <si>
+    <t>2004M10</t>
+  </si>
+  <si>
+    <t>2004M11</t>
+  </si>
+  <si>
+    <t>2004M12</t>
+  </si>
+  <si>
+    <t>2005M01</t>
+  </si>
+  <si>
+    <t>2005M02</t>
+  </si>
+  <si>
+    <t>2005M03</t>
+  </si>
+  <si>
+    <t>2005M04</t>
+  </si>
+  <si>
+    <t>2005M05</t>
+  </si>
+  <si>
+    <t>2005M06</t>
+  </si>
+  <si>
+    <t>2005M07</t>
+  </si>
+  <si>
+    <t>2005M08</t>
+  </si>
+  <si>
+    <t>2005M09</t>
+  </si>
+  <si>
+    <t>2005M10</t>
+  </si>
+  <si>
+    <t>2005M11</t>
+  </si>
+  <si>
+    <t>2005M12</t>
+  </si>
+  <si>
+    <t>2006M01</t>
+  </si>
+  <si>
+    <t>2006M02</t>
+  </si>
+  <si>
+    <t>2006M03</t>
+  </si>
+  <si>
+    <t>2006M04</t>
+  </si>
+  <si>
+    <t>2006M05</t>
+  </si>
+  <si>
+    <t>2006M06</t>
+  </si>
+  <si>
+    <t>2006M07</t>
+  </si>
+  <si>
+    <t>2006M08</t>
+  </si>
+  <si>
+    <t>2006M09</t>
+  </si>
+  <si>
+    <t>2006M10</t>
+  </si>
+  <si>
+    <t>2006M11</t>
+  </si>
+  <si>
+    <t>2006M12</t>
+  </si>
+  <si>
+    <t>2007M01</t>
+  </si>
+  <si>
+    <t>2007M02</t>
+  </si>
+  <si>
+    <t>2007M03</t>
+  </si>
+  <si>
+    <t>2007M04</t>
+  </si>
+  <si>
+    <t>2007M05</t>
+  </si>
+  <si>
+    <t>2007M06</t>
+  </si>
+  <si>
+    <t>2007M07</t>
+  </si>
+  <si>
+    <t>2007M08</t>
+  </si>
+  <si>
+    <t>2007M09</t>
+  </si>
+  <si>
+    <t>2007M10</t>
+  </si>
+  <si>
+    <t>2007M11</t>
+  </si>
+  <si>
+    <t>2007M12</t>
+  </si>
+  <si>
+    <t>2008M01</t>
+  </si>
+  <si>
+    <t>2008M02</t>
+  </si>
+  <si>
+    <t>2008M03</t>
+  </si>
+  <si>
+    <t>2008M04</t>
+  </si>
+  <si>
+    <t>2008M05</t>
+  </si>
+  <si>
+    <t>2008M06</t>
+  </si>
+  <si>
+    <t>2008M07</t>
+  </si>
+  <si>
+    <t>2008M08</t>
+  </si>
+  <si>
+    <t>2008M09</t>
+  </si>
+  <si>
+    <t>2008M10</t>
+  </si>
+  <si>
+    <t>2008M11</t>
+  </si>
+  <si>
+    <t>2008M12</t>
+  </si>
+  <si>
+    <t>2009M01</t>
+  </si>
+  <si>
+    <t>2009M02</t>
+  </si>
+  <si>
+    <t>2009M03</t>
+  </si>
+  <si>
+    <t>2009M04</t>
+  </si>
+  <si>
+    <t>2009M05</t>
+  </si>
+  <si>
+    <t>2009M06</t>
+  </si>
+  <si>
+    <t>2009M07</t>
+  </si>
+  <si>
+    <t>2009M08</t>
+  </si>
+  <si>
+    <t>2009M09</t>
+  </si>
+  <si>
+    <t>2009M10</t>
+  </si>
+  <si>
+    <t>2009M11</t>
+  </si>
+  <si>
+    <t>2009M12</t>
+  </si>
+  <si>
+    <t>2010M01</t>
   </si>
 </sst>
 </file>
@@ -439,16 +730,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C29B3E3-A90D-419A-8D53-0F04D2F51624}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFAF0DC-46BC-4AB6-9BA9-26ABD7BCC328}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C98"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="19.7109375" style="1"/>
+    <col min="1" max="16384" width="18.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
@@ -466,8 +757,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>199201</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>182296.935</v>
@@ -476,12 +767,12 @@
         <v>16840.375</v>
       </c>
       <c r="D2" s="2">
-        <v>18.208500000000001</v>
+        <v>182085</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>199202</v>
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>193511.58</v>
@@ -490,12 +781,12 @@
         <v>12864.355</v>
       </c>
       <c r="D3" s="2">
-        <v>16.914999999999999</v>
+        <v>169150</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>199203</v>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>175297.11</v>
@@ -504,12 +795,12 @@
         <v>12114.125</v>
       </c>
       <c r="D4" s="2">
-        <v>17.2135</v>
+        <v>172135</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>199204</v>
+      <c r="A5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>178023.41</v>
@@ -518,12 +809,12 @@
         <v>10068.405000000001</v>
       </c>
       <c r="D5" s="2">
-        <v>16.616499999999998</v>
+        <v>166164.99999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>199205</v>
+      <c r="A6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>157768.19500000001</v>
@@ -532,12 +823,12 @@
         <v>10957.934999999999</v>
       </c>
       <c r="D6" s="2">
-        <v>15.323</v>
+        <v>153230</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>199206</v>
+      <c r="A7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>159826.85</v>
@@ -546,12 +837,12 @@
         <v>9967.91</v>
       </c>
       <c r="D7" s="2">
-        <v>14.925000000000001</v>
+        <v>149250</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>199207</v>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>171510.13999999998</v>
@@ -560,12 +851,12 @@
         <v>10996.74</v>
       </c>
       <c r="D8" s="2">
-        <v>16.019500000000001</v>
+        <v>160195</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>199208</v>
+      <c r="A9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>177860.23</v>
@@ -574,12 +865,12 @@
         <v>13112.11</v>
       </c>
       <c r="D9" s="2">
-        <v>17.2135</v>
+        <v>172135</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>199209</v>
+      <c r="A10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>196429.91500000001</v>
@@ -588,12 +879,12 @@
         <v>11740.004999999999</v>
       </c>
       <c r="D10" s="2">
-        <v>17.810499999999998</v>
+        <v>178104.99999999997</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>199210</v>
+      <c r="A11" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>200499.465</v>
@@ -602,12 +893,12 @@
         <v>12249.445</v>
       </c>
       <c r="D11" s="2">
-        <v>18.108999999999998</v>
+        <v>181089.99999999997</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>199211</v>
+      <c r="A12" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <v>182537.72500000001</v>
@@ -616,12 +907,12 @@
         <v>11811.645</v>
       </c>
       <c r="D12" s="2">
-        <v>16.119</v>
+        <v>161190</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>199212</v>
+      <c r="A13" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>195991.12</v>
@@ -630,12 +921,12 @@
         <v>13771.795</v>
       </c>
       <c r="D13" s="2">
-        <v>18.507000000000001</v>
+        <v>185070</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>199301</v>
+      <c r="A14" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>164773.99</v>
@@ -644,12 +935,12 @@
         <v>12279.295</v>
       </c>
       <c r="D14" s="2">
-        <v>17.014500000000002</v>
+        <v>170145.00000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>199302</v>
+      <c r="A15" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <v>179973.61</v>
@@ -658,12 +949,12 @@
         <v>12666.35</v>
       </c>
       <c r="D15" s="2">
-        <v>16.716000000000001</v>
+        <v>167160</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>199303</v>
+      <c r="A16" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <v>200005.94500000001</v>
@@ -672,12 +963,12 @@
         <v>15229.47</v>
       </c>
       <c r="D16" s="2">
-        <v>18.407499999999999</v>
+        <v>184075</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>199304</v>
+      <c r="A17" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>197600.035</v>
@@ -686,12 +977,12 @@
         <v>12692.22</v>
       </c>
       <c r="D17" s="2">
-        <v>17.810499999999998</v>
+        <v>178104.99999999997</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>199305</v>
+      <c r="A18" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <v>182842.19500000001</v>
@@ -700,12 +991,12 @@
         <v>11998.705</v>
       </c>
       <c r="D18" s="2">
-        <v>16.914999999999999</v>
+        <v>169150</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>199306</v>
+      <c r="A19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <v>185532.67499999999</v>
@@ -714,12 +1005,12 @@
         <v>14042.434999999999</v>
       </c>
       <c r="D19" s="2">
-        <v>18.407499999999999</v>
+        <v>184075</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>199307</v>
+      <c r="A20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="2">
         <v>188795.28</v>
@@ -728,12 +1019,12 @@
         <v>15565.78</v>
       </c>
       <c r="D20" s="2">
-        <v>19.103999999999999</v>
+        <v>191040</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>199308</v>
+      <c r="A21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B21" s="2">
         <v>231354.41500000001</v>
@@ -742,12 +1033,12 @@
         <v>17898.060000000001</v>
       </c>
       <c r="D21" s="2">
-        <v>22.088999999999999</v>
+        <v>220890</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>199309</v>
+      <c r="A22" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B22" s="2">
         <v>230609.16</v>
@@ -756,12 +1047,12 @@
         <v>15224.495000000001</v>
       </c>
       <c r="D22" s="2">
-        <v>21.292999999999999</v>
+        <v>212930</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>199310</v>
+      <c r="A23" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="2">
         <v>226637.12</v>
@@ -770,12 +1061,12 @@
         <v>14999.625</v>
       </c>
       <c r="D23" s="2">
-        <v>20.198499999999999</v>
+        <v>201985</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>199311</v>
+      <c r="A24" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B24" s="2">
         <v>218658.215</v>
@@ -784,12 +1075,12 @@
         <v>16634.41</v>
       </c>
       <c r="D24" s="2">
-        <v>20.895</v>
+        <v>208950</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>199312</v>
+      <c r="A25" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B25" s="2">
         <v>229289.79</v>
@@ -798,12 +1089,12 @@
         <v>16144.87</v>
       </c>
       <c r="D25" s="2">
-        <v>23.3825</v>
+        <v>233825</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>199401</v>
+      <c r="A26" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B26" s="2">
         <v>212128.03</v>
@@ -812,12 +1103,12 @@
         <v>18195.564999999999</v>
       </c>
       <c r="D26" s="2">
-        <v>21.790499999999998</v>
+        <v>217904.99999999997</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>199402</v>
+      <c r="A27" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B27" s="2">
         <v>207412.72500000001</v>
@@ -826,12 +1117,12 @@
         <v>18311.98</v>
       </c>
       <c r="D27" s="2">
-        <v>19.8005</v>
+        <v>198005</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>199403</v>
+      <c r="A28" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B28" s="2">
         <v>230438.02</v>
@@ -840,12 +1131,12 @@
         <v>19634.334999999999</v>
       </c>
       <c r="D28" s="2">
-        <v>23.3825</v>
+        <v>233825</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>199404</v>
+      <c r="A29" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B29" s="2">
         <v>219274.12</v>
@@ -854,12 +1145,12 @@
         <v>18001.54</v>
       </c>
       <c r="D29" s="2">
-        <v>22.288</v>
+        <v>222880</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>199405</v>
+      <c r="A30" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B30" s="2">
         <v>233841.91500000001</v>
@@ -868,12 +1159,12 @@
         <v>18045.32</v>
       </c>
       <c r="D30" s="2">
-        <v>22.586500000000001</v>
+        <v>225865</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>199406</v>
+      <c r="A31" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B31" s="2">
         <v>232213.1</v>
@@ -882,12 +1173,12 @@
         <v>18958.73</v>
       </c>
       <c r="D31" s="2">
-        <v>23.3825</v>
+        <v>233825</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>199407</v>
+      <c r="A32" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B32" s="2">
         <v>245490.38</v>
@@ -896,12 +1187,12 @@
         <v>17130.915000000001</v>
       </c>
       <c r="D32" s="2">
-        <v>23.88</v>
+        <v>238800</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>199408</v>
+      <c r="A33" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B33" s="2">
         <v>298457.21500000003</v>
@@ -910,12 +1201,12 @@
         <v>22888.98</v>
       </c>
       <c r="D33" s="2">
-        <v>27.462</v>
+        <v>274620</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>199409</v>
+      <c r="A34" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B34" s="2">
         <v>315423.95500000002</v>
@@ -924,12 +1215,12 @@
         <v>23087.98</v>
       </c>
       <c r="D34" s="2">
-        <v>29.651</v>
+        <v>296510</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>199410</v>
+      <c r="A35" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B35" s="2">
         <v>319198.98499999999</v>
@@ -938,12 +1229,12 @@
         <v>23494.935000000001</v>
       </c>
       <c r="D35" s="2">
-        <v>29.9495</v>
+        <v>299495</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>199411</v>
+      <c r="A36" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B36" s="2">
         <v>332088.21500000003</v>
@@ -952,12 +1243,12 @@
         <v>18800.525000000001</v>
       </c>
       <c r="D36" s="2">
-        <v>29.352499999999999</v>
+        <v>293525</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>199412</v>
+      <c r="A37" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B37" s="2">
         <v>317348.28499999997</v>
@@ -966,12 +1257,12 @@
         <v>20918.88</v>
       </c>
       <c r="D37" s="2">
-        <v>31.044</v>
+        <v>310440</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>199501</v>
+      <c r="A38" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B38" s="2">
         <v>290797.70500000002</v>
@@ -980,12 +1271,12 @@
         <v>25978.454999999998</v>
       </c>
       <c r="D38" s="2">
-        <v>28.655999999999999</v>
+        <v>286560</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>199502</v>
+      <c r="A39" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B39" s="2">
         <v>284260.55499999999</v>
@@ -994,12 +1285,12 @@
         <v>23444.19</v>
       </c>
       <c r="D39" s="2">
-        <v>27.064</v>
+        <v>270640</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>199503</v>
+      <c r="A40" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B40" s="2">
         <v>313637.93</v>
@@ -1008,12 +1299,12 @@
         <v>24568.54</v>
       </c>
       <c r="D40" s="2">
-        <v>29.651</v>
+        <v>296510</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>199504</v>
+      <c r="A41" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B41" s="2">
         <v>291588.73</v>
@@ -1022,12 +1313,12 @@
         <v>24954.6</v>
       </c>
       <c r="D41" s="2">
-        <v>28.058999999999997</v>
+        <v>280590</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>199505</v>
+      <c r="A42" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B42" s="2">
         <v>325217.74</v>
@@ -1036,12 +1327,12 @@
         <v>23381.505000000001</v>
       </c>
       <c r="D42" s="2">
-        <v>32.138500000000001</v>
+        <v>321385</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>199506</v>
+      <c r="A43" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B43" s="2">
         <v>295052.32500000001</v>
@@ -1050,12 +1341,12 @@
         <v>26346.605</v>
       </c>
       <c r="D43" s="2">
-        <v>29.253</v>
+        <v>292530</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>199507</v>
+      <c r="A44" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B44" s="2">
         <v>301086.005</v>
@@ -1064,12 +1355,12 @@
         <v>25522.744999999999</v>
       </c>
       <c r="D44" s="2">
-        <v>28.5565</v>
+        <v>285565</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>199508</v>
+      <c r="A45" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B45" s="2">
         <v>334245.375</v>
@@ -1078,12 +1369,12 @@
         <v>26737.64</v>
       </c>
       <c r="D45" s="2">
-        <v>31.641000000000002</v>
+        <v>316410</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>199509</v>
+      <c r="A46" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B46" s="2">
         <v>326952.02500000002</v>
@@ -1092,12 +1383,12 @@
         <v>26273.97</v>
       </c>
       <c r="D46" s="2">
-        <v>30.447000000000003</v>
+        <v>304470</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>199510</v>
+      <c r="A47" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B47" s="2">
         <v>337230.375</v>
@@ -1106,12 +1397,12 @@
         <v>26431.18</v>
       </c>
       <c r="D47" s="2">
-        <v>31.939500000000002</v>
+        <v>319395</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>199511</v>
+      <c r="A48" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B48" s="2">
         <v>326236.62</v>
@@ -1120,12 +1411,12 @@
         <v>27058.03</v>
       </c>
       <c r="D48" s="2">
-        <v>30.048999999999999</v>
+        <v>300490</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>199512</v>
+      <c r="A49" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B49" s="2">
         <v>304543.63</v>
@@ -1134,12 +1425,12 @@
         <v>24682.965</v>
       </c>
       <c r="D49" s="2">
-        <v>29.352499999999999</v>
+        <v>293525</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>199601</v>
+      <c r="A50" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B50" s="2">
         <v>305943.59499999997</v>
@@ -1148,12 +1439,12 @@
         <v>27040.12</v>
       </c>
       <c r="D50" s="2">
-        <v>28.655999999999999</v>
+        <v>286560</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>199602</v>
+      <c r="A51" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B51" s="2">
         <v>294904.07</v>
@@ -1162,12 +1453,12 @@
         <v>24648.14</v>
       </c>
       <c r="D51" s="2">
-        <v>26.168500000000002</v>
+        <v>261685.00000000003</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>199603</v>
+      <c r="A52" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B52" s="2">
         <v>297051.27999999997</v>
@@ -1176,12 +1467,12 @@
         <v>26213.275000000001</v>
       </c>
       <c r="D52" s="2">
-        <v>28.357499999999998</v>
+        <v>283575</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>199604</v>
+      <c r="A53" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B53" s="2">
         <v>293804.59499999997</v>
@@ -1190,12 +1481,12 @@
         <v>25927.71</v>
       </c>
       <c r="D53" s="2">
-        <v>25.173500000000001</v>
+        <v>251735</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>199605</v>
+      <c r="A54" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B54" s="2">
         <v>320106.42499999999</v>
@@ -1204,12 +1495,12 @@
         <v>32171.334999999999</v>
       </c>
       <c r="D54" s="2">
-        <v>27.959500000000002</v>
+        <v>279595</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>199606</v>
+      <c r="A55" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B55" s="2">
         <v>288392.78999999998</v>
@@ -1218,12 +1509,12 @@
         <v>28324.665000000001</v>
       </c>
       <c r="D55" s="2">
-        <v>24.775499999999997</v>
+        <v>247754.99999999997</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>199607</v>
+      <c r="A56" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B56" s="2">
         <v>323585.94</v>
@@ -1232,12 +1523,12 @@
         <v>30621.125</v>
       </c>
       <c r="D56" s="2">
-        <v>27.163499999999999</v>
+        <v>271635</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>199608</v>
+      <c r="A57" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B57" s="2">
         <v>334370.745</v>
@@ -1246,12 +1537,12 @@
         <v>31785.275000000001</v>
       </c>
       <c r="D57" s="2">
-        <v>29.153500000000001</v>
+        <v>291535</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>199609</v>
+      <c r="A58" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B58" s="2">
         <v>332946.90000000002</v>
@@ -1260,12 +1551,12 @@
         <v>30335.56</v>
       </c>
       <c r="D58" s="2">
-        <v>28.257999999999999</v>
+        <v>282580</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>199610</v>
+      <c r="A59" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B59" s="2">
         <v>349838.02</v>
@@ -1274,12 +1565,12 @@
         <v>31505.68</v>
       </c>
       <c r="D59" s="2">
-        <v>31.1435</v>
+        <v>311435</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>199611</v>
+      <c r="A60" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B60" s="2">
         <v>334126.96999999997</v>
@@ -1288,12 +1579,12 @@
         <v>33907.61</v>
       </c>
       <c r="D60" s="2">
-        <v>29.750499999999999</v>
+        <v>297505</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>199612</v>
+      <c r="A61" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B61" s="2">
         <v>344088.91</v>
@@ -1302,12 +1593,12 @@
         <v>29000.27</v>
       </c>
       <c r="D61" s="2">
-        <v>32.437000000000005</v>
+        <v>324370.00000000006</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>199701</v>
+      <c r="A62" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B62" s="2">
         <v>349437.03499999997</v>
@@ -1316,12 +1607,12 @@
         <v>36938.379999999997</v>
       </c>
       <c r="D62" s="2">
-        <v>33.83</v>
+        <v>338300</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>199702</v>
+      <c r="A63" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B63" s="2">
         <v>326781.88</v>
@@ -1330,12 +1621,12 @@
         <v>34497.644999999997</v>
       </c>
       <c r="D63" s="2">
-        <v>30.3475</v>
+        <v>303475</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>199703</v>
+      <c r="A64" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B64" s="2">
         <v>312836.95500000002</v>
@@ -1344,12 +1635,12 @@
         <v>30138.55</v>
       </c>
       <c r="D64" s="2">
-        <v>30.048999999999999</v>
+        <v>300490</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>199704</v>
+      <c r="A65" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B65" s="2">
         <v>335137.89</v>
@@ -1358,12 +1649,12 @@
         <v>25567.52</v>
       </c>
       <c r="D65" s="2">
-        <v>31.641000000000002</v>
+        <v>316410</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>199705</v>
+      <c r="A66" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B66" s="2">
         <v>344354.57500000001</v>
@@ -1372,12 +1663,12 @@
         <v>16196.609999999999</v>
       </c>
       <c r="D66" s="2">
-        <v>31.939500000000002</v>
+        <v>319395</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>199706</v>
+      <c r="A67" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B67" s="2">
         <v>325049.58500000002</v>
@@ -1386,12 +1677,12 @@
         <v>27131.66</v>
       </c>
       <c r="D67" s="2">
-        <v>30.546499999999998</v>
+        <v>305465</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>199707</v>
+      <c r="A68" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B68" s="2">
         <v>344714.76500000001</v>
@@ -1400,12 +1691,12 @@
         <v>40355.21</v>
       </c>
       <c r="D68" s="2">
-        <v>32.635999999999996</v>
+        <v>326359.99999999994</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>199708</v>
+      <c r="A69" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B69" s="2">
         <v>371620.56</v>
@@ -1414,12 +1705,12 @@
         <v>34718.534999999996</v>
       </c>
       <c r="D69" s="2">
-        <v>33.929500000000004</v>
+        <v>339295.00000000006</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>199709</v>
+      <c r="A70" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B70" s="2">
         <v>389571.35499999998</v>
@@ -1428,12 +1719,12 @@
         <v>35085.69</v>
       </c>
       <c r="D70" s="2">
-        <v>37.3125</v>
+        <v>373125</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>199710</v>
+      <c r="A71" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B71" s="2">
         <v>401778.01500000001</v>
@@ -1442,12 +1733,12 @@
         <v>34337.449999999997</v>
       </c>
       <c r="D71" s="2">
-        <v>42.088499999999996</v>
+        <v>420884.99999999994</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>199711</v>
+      <c r="A72" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B72" s="2">
         <v>373071.27</v>
@@ -1456,12 +1747,12 @@
         <v>33308.620000000003</v>
       </c>
       <c r="D72" s="2">
-        <v>37.3125</v>
+        <v>373125</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>199712</v>
+      <c r="A73" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B73" s="2">
         <v>393263.8</v>
@@ -1470,12 +1761,12 @@
         <v>34231.980000000003</v>
       </c>
       <c r="D73" s="2">
-        <v>36.317500000000003</v>
+        <v>363175</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
-        <v>199801</v>
+      <c r="A74" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B74" s="2">
         <v>359392.01</v>
@@ -1484,12 +1775,12 @@
         <v>32731.52</v>
       </c>
       <c r="D74" s="2">
-        <v>34.924500000000002</v>
+        <v>349245</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
-        <v>199802</v>
+      <c r="A75" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B75" s="2">
         <v>331319.08</v>
@@ -1498,12 +1789,12 @@
         <v>33138.474999999999</v>
       </c>
       <c r="D75" s="2">
-        <v>32.635999999999996</v>
+        <v>326359.99999999994</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
-        <v>199803</v>
+      <c r="A76" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B76" s="2">
         <v>357980.10499999998</v>
@@ -1512,12 +1803,12 @@
         <v>30889.775000000001</v>
       </c>
       <c r="D76" s="2">
-        <v>35.222999999999999</v>
+        <v>352230</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
-        <v>199804</v>
+      <c r="A77" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B77" s="2">
         <v>329527.08500000002</v>
@@ -1526,12 +1817,12 @@
         <v>28343.57</v>
       </c>
       <c r="D77" s="2">
-        <v>32.238</v>
+        <v>322380</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
-        <v>199805</v>
+      <c r="A78" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B78" s="2">
         <v>320388.01</v>
@@ -1540,12 +1831,12 @@
         <v>23565.579999999998</v>
       </c>
       <c r="D78" s="2">
-        <v>30.944500000000001</v>
+        <v>309445</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
-        <v>199806</v>
+      <c r="A79" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B79" s="2">
         <v>342333.73</v>
@@ -1554,12 +1845,12 @@
         <v>33381.254999999997</v>
       </c>
       <c r="D79" s="2">
-        <v>33.332500000000003</v>
+        <v>333325.00000000006</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>199807</v>
+      <c r="A80" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B80" s="2">
         <v>370256.41499999998</v>
@@ -1568,12 +1859,12 @@
         <v>35896.614999999998</v>
       </c>
       <c r="D80" s="2">
-        <v>35.919499999999999</v>
+        <v>359195</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>199808</v>
+      <c r="A81" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B81" s="2">
         <v>423605.33</v>
@@ -1582,12 +1873,12 @@
         <v>36607.044999999998</v>
       </c>
       <c r="D81" s="2">
-        <v>38.009</v>
+        <v>380090</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>199809</v>
+      <c r="A82" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B82" s="2">
         <v>395782.14500000002</v>
@@ -1596,12 +1887,12 @@
         <v>38563.214999999997</v>
       </c>
       <c r="D82" s="2">
-        <v>37.3125</v>
+        <v>373125</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
-        <v>199810</v>
+      <c r="A83" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B83" s="2">
         <v>351235.995</v>
@@ -1610,12 +1901,12 @@
         <v>32672.814999999999</v>
       </c>
       <c r="D83" s="2">
-        <v>36.417000000000002</v>
+        <v>364170</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>199811</v>
+      <c r="A84" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B84" s="2">
         <v>346403.27999999997</v>
@@ -1624,12 +1915,12 @@
         <v>25053.105</v>
       </c>
       <c r="D84" s="2">
-        <v>34.228000000000002</v>
+        <v>342280</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>199812</v>
+      <c r="A85" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B85" s="2">
         <v>341543.7</v>
@@ -1638,12 +1929,12 @@
         <v>23017.334999999999</v>
       </c>
       <c r="D85" s="2">
-        <v>32.138500000000001</v>
+        <v>321385</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>199901</v>
+      <c r="A86" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B86" s="2">
         <v>309646.98499999999</v>
@@ -1652,12 +1943,12 @@
         <v>29746.52</v>
       </c>
       <c r="D86" s="2">
-        <v>30.3475</v>
+        <v>303475</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>199902</v>
+      <c r="A87" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B87" s="2">
         <v>271692.71000000002</v>
@@ -1666,12 +1957,12 @@
         <v>25631.200000000001</v>
       </c>
       <c r="D87" s="2">
-        <v>27.462</v>
+        <v>274620</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>199903</v>
+      <c r="A88" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B88" s="2">
         <v>329841.505</v>
@@ -1680,12 +1971,12 @@
         <v>27817.215</v>
       </c>
       <c r="D88" s="2">
-        <v>30.646000000000001</v>
+        <v>306460</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>199904</v>
+      <c r="A89" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B89" s="2">
         <v>283531.21999999997</v>
@@ -1694,12 +1985,12 @@
         <v>23929.75</v>
       </c>
       <c r="D89" s="2">
-        <v>27.362500000000001</v>
+        <v>273625</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>199905</v>
+      <c r="A90" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B90" s="2">
         <v>276831.88500000001</v>
@@ -1708,12 +1999,12 @@
         <v>24543.665000000001</v>
       </c>
       <c r="D90" s="2">
-        <v>24.974500000000003</v>
+        <v>249745.00000000003</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>199906</v>
+      <c r="A91" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B91" s="2">
         <v>284278.46500000003</v>
@@ -1722,12 +2013,12 @@
         <v>25373.494999999999</v>
       </c>
       <c r="D91" s="2">
-        <v>26.267999999999997</v>
+        <v>262680</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>199907</v>
+      <c r="A92" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B92" s="2">
         <v>298833.32500000001</v>
@@ -1736,12 +2027,12 @@
         <v>27083.9</v>
       </c>
       <c r="D92" s="2">
-        <v>28.058999999999997</v>
+        <v>280590</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
-        <v>199908</v>
+      <c r="A93" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B93" s="2">
         <v>322651.63500000001</v>
@@ -1750,12 +2041,12 @@
         <v>32455.904999999999</v>
       </c>
       <c r="D93" s="2">
-        <v>31.242999999999999</v>
+        <v>312430</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
-        <v>199909</v>
+      <c r="A94" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B94" s="2">
         <v>337450.27</v>
@@ -1764,12 +2055,12 @@
         <v>34818.034999999996</v>
       </c>
       <c r="D94" s="2">
-        <v>32.635999999999996</v>
+        <v>326359.99999999994</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
-        <v>199910</v>
+      <c r="A95" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B95" s="2">
         <v>341783.495</v>
@@ -1778,12 +2069,12 @@
         <v>34415.06</v>
       </c>
       <c r="D95" s="2">
-        <v>35.919499999999999</v>
+        <v>359195</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
-        <v>199911</v>
+      <c r="A96" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B96" s="2">
         <v>351843.94</v>
@@ -1792,12 +2083,12 @@
         <v>30434.064999999999</v>
       </c>
       <c r="D96" s="2">
-        <v>35.1235</v>
+        <v>351235</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
-        <v>199912</v>
+      <c r="A97" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B97" s="2">
         <v>348840.03499999997</v>
@@ -1806,12 +2097,12 @@
         <v>27806.27</v>
       </c>
       <c r="D97" s="2">
-        <v>32.635999999999996</v>
+        <v>326359.99999999994</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
-        <v>200001</v>
+      <c r="A98" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B98" s="2">
         <v>310969.34000000003</v>
@@ -1820,7 +2111,7 @@
         <v>31234.044999999998</v>
       </c>
       <c r="D98" s="2">
-        <v>31.84</v>
+        <v>318400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>